<commit_message>
Npm modulok telepítése, listening
</commit_message>
<xml_diff>
--- a/docs/Adatbázis.xlsx
+++ b/docs/Adatbázis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>tábla neve</t>
   </si>
@@ -87,9 +87,6 @@
     <t>img</t>
   </si>
   <si>
-    <t>&gt;:(</t>
-  </si>
-  <si>
     <t>datum</t>
   </si>
   <si>
@@ -108,19 +105,16 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>kovetesek</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>kovetett_user</t>
-  </si>
-  <si>
-    <t>kommentek</t>
-  </si>
-  <si>
-    <t>tartalom</t>
+    <t>kovetett_user_id</t>
+  </si>
+  <si>
+    <t>follows</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -444,17 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -562,162 +556,166 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="B13:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A2:A34"/>
+    <mergeCell ref="B23:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>